<commit_message>
updated the data file
</commit_message>
<xml_diff>
--- a/resources/Automation_Data.xlsx
+++ b/resources/Automation_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jjill-my.sharepoint.com/personal/nikhitha_muthukur_jjill_com/Documents/Automation/Projects/JJillTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04140DD3-1397-4303-9A95-E8163D3C4270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{04140DD3-1397-4303-9A95-E8163D3C4270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E874C2DD-6B66-40C3-8F5B-227975849E92}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="1" activeTab="3" xr2:uid="{6BFA5E0A-9DDB-4471-A408-EA685EED7E6E}"/>
   </bookViews>
@@ -168,9 +168,6 @@
     <t>229881</t>
   </si>
   <si>
-    <t>22988145NS</t>
-  </si>
-  <si>
     <t>22988147ZL</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>22988145NL</t>
   </si>
 </sst>
 </file>
@@ -868,7 +868,7 @@
   <dimension ref="A1:XFD6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17303,7 +17303,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:16384" x14ac:dyDescent="0.35">
@@ -17311,7 +17311,7 @@
         <v>42</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>45</v>
@@ -17322,10 +17322,10 @@
         <v>43</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added code to GIT
</commit_message>
<xml_diff>
--- a/resources/Automation_Data.xlsx
+++ b/resources/Automation_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jjill-my.sharepoint.com/personal/nikhitha_muthukur_jjill_com/Documents/Automation/Projects/JJillTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitkhitha.kuthukur\OneDrive - J.Jill\Automation\Projects\JJillTest\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{04140DD3-1397-4303-9A95-E8163D3C4270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E874C2DD-6B66-40C3-8F5B-227975849E92}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD08CB2D-C9B7-4109-B74D-A178235C2807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="1" activeTab="3" xr2:uid="{6BFA5E0A-9DDB-4471-A408-EA685EED7E6E}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
   <si>
     <t>Scenario</t>
   </si>
@@ -150,9 +150,6 @@
     <t>CTL</t>
   </si>
   <si>
-    <t>234041</t>
-  </si>
-  <si>
     <t>BackOrdered</t>
   </si>
   <si>
@@ -165,26 +162,65 @@
     <t>3</t>
   </si>
   <si>
-    <t>229881</t>
-  </si>
-  <si>
-    <t>22988147ZL</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>22988145NL</t>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>SizeType</t>
+  </si>
+  <si>
+    <t>Petite</t>
+  </si>
+  <si>
+    <t>235061</t>
+  </si>
+  <si>
+    <t>234281</t>
+  </si>
+  <si>
+    <t>clearwater multi</t>
+  </si>
+  <si>
+    <t>XLP</t>
+  </si>
+  <si>
+    <t>Tall</t>
+  </si>
+  <si>
+    <t>sea/vintage canvas</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>239283</t>
+  </si>
+  <si>
+    <t>navy blue</t>
+  </si>
+  <si>
+    <t>1X</t>
+  </si>
+  <si>
+    <t>Women's</t>
+  </si>
+  <si>
+    <t>236301</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +248,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF474747"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -227,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -261,12 +303,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,6 +361,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -865,20 +924,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA23885-4FA5-45F3-86BB-5039FDA0F69E}">
-  <dimension ref="A1:XFD6"/>
+  <dimension ref="A1:XFD7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.1796875" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -888,9 +948,15 @@
       <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -902,6 +968,9 @@
       <c r="C2" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -911,12 +980,12 @@
         <v>34</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="17"/>
       <c r="H3" s="4"/>
       <c r="I3" s="6"/>
       <c r="J3" s="3"/>
@@ -17297,36 +17366,66 @@
     </row>
     <row r="4" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>46</v>
+        <v>61</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
+      <c r="D6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.35">
+      <c r="C7" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>